<commit_message>
fill in missing frag_id numbers
</commit_message>
<xml_diff>
--- a/data/tle/2019-10-17_ALL.xlsx
+++ b/data/tle/2019-10-17_ALL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/bsrte/data/tle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947EEC3F-2E4E-B145-89B5-C3B9361FC166}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6963254B-A740-984E-9F55-ECB3D07534FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="23000" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -935,8 +935,8 @@
   <dimension ref="A1:I571"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A564" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E282" sqref="E282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4432,6 +4432,9 @@
       <c r="D152">
         <v>53</v>
       </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
       <c r="F152" t="s">
         <v>59</v>
       </c>
@@ -4452,6 +4455,9 @@
       <c r="D153">
         <v>53</v>
       </c>
+      <c r="E153">
+        <v>2</v>
+      </c>
       <c r="F153" t="s">
         <v>60</v>
       </c>
@@ -4472,6 +4478,9 @@
       <c r="D154">
         <v>53</v>
       </c>
+      <c r="E154">
+        <v>3</v>
+      </c>
       <c r="F154" t="s">
         <v>61</v>
       </c>
@@ -4492,6 +4501,9 @@
       <c r="D155">
         <v>53</v>
       </c>
+      <c r="E155">
+        <v>4</v>
+      </c>
       <c r="F155" t="s">
         <v>33</v>
       </c>
@@ -4512,6 +4524,9 @@
       <c r="D156">
         <v>53</v>
       </c>
+      <c r="E156">
+        <v>5</v>
+      </c>
       <c r="F156" t="s">
         <v>62</v>
       </c>
@@ -7232,6 +7247,9 @@
       <c r="D277">
         <v>49</v>
       </c>
+      <c r="E277">
+        <v>1</v>
+      </c>
       <c r="F277" t="s">
         <v>87</v>
       </c>
@@ -7249,6 +7267,9 @@
       <c r="D278">
         <v>49</v>
       </c>
+      <c r="E278">
+        <v>2</v>
+      </c>
       <c r="F278" t="s">
         <v>89</v>
       </c>
@@ -7266,6 +7287,9 @@
       <c r="D279">
         <v>49</v>
       </c>
+      <c r="E279">
+        <v>3</v>
+      </c>
       <c r="F279" t="s">
         <v>87</v>
       </c>
@@ -7283,6 +7307,9 @@
       <c r="D280">
         <v>49</v>
       </c>
+      <c r="E280">
+        <v>4</v>
+      </c>
       <c r="F280" t="s">
         <v>28</v>
       </c>
@@ -7299,6 +7326,9 @@
       </c>
       <c r="D281">
         <v>49</v>
+      </c>
+      <c r="E281">
+        <v>5</v>
       </c>
       <c r="F281" t="s">
         <v>90</v>

</xml_diff>